<commit_message>
fixing CRX format error
</commit_message>
<xml_diff>
--- a/notebooks/CRX/input/CRX_CORD2_individuals.xlsx
+++ b/notebooks/CRX/input/CRX_CORD2_individuals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin/GIT/phenopacket-store/notebooks/CRX/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F706BC05-EBC4-E942-AC95-8D16E74C1536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB36F7F6-EDF5-CA45-9F19-C647E90E6C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="33680" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29840" yWindow="6520" windowWidth="42600" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -573,7 +573,7 @@
   <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>